<commit_message>
Tabla inscripcion moto Corrientes
</commit_message>
<xml_diff>
--- a/script_DNRPA/registroInscripcionAutoCorientes.xlsx
+++ b/script_DNRPA/registroInscripcionAutoCorientes.xlsx
@@ -393,7 +393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,644 +484,726 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
+          <t>5016 - CORRIENTES N° 5</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>5017 - ITUZAINGO N° 2</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>TOTAL</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>41640</v>
+        <v>44562</v>
       </c>
       <c r="B2" t="n">
-        <v>178</v>
+        <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>364</v>
+        <v>78</v>
       </c>
       <c r="D2" t="n">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="E2" t="n">
-        <v>238</v>
+        <v>53</v>
       </c>
       <c r="F2" t="n">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="G2" t="n">
-        <v>169</v>
+        <v>62</v>
       </c>
       <c r="H2" t="n">
-        <v>136</v>
+        <v>39</v>
       </c>
       <c r="I2" t="n">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="J2" t="n">
-        <v>405</v>
+        <v>54</v>
       </c>
       <c r="K2" t="n">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="L2" t="n">
-        <v>295</v>
+        <v>89</v>
       </c>
       <c r="M2" t="n">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="N2" t="n">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="O2" t="n">
-        <v>232</v>
+        <v>83</v>
       </c>
       <c r="P2" t="n">
-        <v>263</v>
+        <v>132</v>
       </c>
       <c r="Q2" t="n">
-        <v>2796</v>
+        <v>89</v>
+      </c>
+      <c r="R2" t="n">
+        <v>63</v>
+      </c>
+      <c r="S2" t="n">
+        <v>985</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>41671</v>
+        <v>44593</v>
       </c>
       <c r="B3" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="C3" t="n">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="D3" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E3" t="n">
-        <v>119</v>
+        <v>35</v>
       </c>
       <c r="F3" t="n">
+        <v>25</v>
+      </c>
+      <c r="G3" t="n">
+        <v>63</v>
+      </c>
+      <c r="H3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I3" t="n">
+        <v>37</v>
+      </c>
+      <c r="J3" t="n">
+        <v>34</v>
+      </c>
+      <c r="K3" t="n">
+        <v>36</v>
+      </c>
+      <c r="L3" t="n">
+        <v>34</v>
+      </c>
+      <c r="M3" t="n">
+        <v>16</v>
+      </c>
+      <c r="N3" t="n">
         <v>24</v>
       </c>
-      <c r="G3" t="n">
-        <v>99</v>
-      </c>
-      <c r="H3" t="n">
+      <c r="O3" t="n">
+        <v>56</v>
+      </c>
+      <c r="P3" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q3" t="n">
         <v>70</v>
       </c>
-      <c r="I3" t="n">
-        <v>54</v>
-      </c>
-      <c r="J3" t="n">
-        <v>207</v>
-      </c>
-      <c r="K3" t="n">
-        <v>47</v>
-      </c>
-      <c r="L3" t="n">
-        <v>169</v>
-      </c>
-      <c r="M3" t="n">
-        <v>33</v>
-      </c>
-      <c r="N3" t="n">
-        <v>68</v>
-      </c>
-      <c r="O3" t="n">
-        <v>95</v>
-      </c>
-      <c r="P3" t="n">
-        <v>96</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>1360</v>
+      <c r="R3" t="n">
+        <v>62</v>
+      </c>
+      <c r="S3" t="n">
+        <v>735</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>41699</v>
+        <v>44621</v>
       </c>
       <c r="B4" t="n">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="C4" t="n">
-        <v>182</v>
+        <v>69</v>
       </c>
       <c r="D4" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E4" t="n">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="F4" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G4" t="n">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H4" t="n">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="I4" t="n">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J4" t="n">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="K4" t="n">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="L4" t="n">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="M4" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="N4" t="n">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="O4" t="n">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="P4" t="n">
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="Q4" t="n">
-        <v>1105</v>
+        <v>64</v>
+      </c>
+      <c r="R4" t="n">
+        <v>62</v>
+      </c>
+      <c r="S4" t="n">
+        <v>838</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>41730</v>
+        <v>44652</v>
       </c>
       <c r="B5" t="n">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C5" t="n">
-        <v>184</v>
+        <v>43</v>
       </c>
       <c r="D5" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5" t="n">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="F5" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G5" t="n">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="H5" t="n">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="I5" t="n">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="J5" t="n">
-        <v>154</v>
+        <v>48</v>
       </c>
       <c r="K5" t="n">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="L5" t="n">
-        <v>178</v>
+        <v>39</v>
       </c>
       <c r="M5" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="N5" t="n">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="O5" t="n">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="P5" t="n">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="Q5" t="n">
-        <v>1214</v>
+        <v>49</v>
+      </c>
+      <c r="R5" t="n">
+        <v>64</v>
+      </c>
+      <c r="S5" t="n">
+        <v>667</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>41760</v>
+        <v>44682</v>
       </c>
       <c r="B6" t="n">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" t="n">
-        <v>237</v>
+        <v>81</v>
       </c>
       <c r="D6" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E6" t="n">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="F6" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G6" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H6" t="n">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="I6" t="n">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="J6" t="n">
-        <v>202</v>
+        <v>44</v>
       </c>
       <c r="K6" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="L6" t="n">
-        <v>196</v>
+        <v>44</v>
       </c>
       <c r="M6" t="n">
+        <v>12</v>
+      </c>
+      <c r="N6" t="n">
         <v>31</v>
       </c>
-      <c r="N6" t="n">
-        <v>61</v>
-      </c>
       <c r="O6" t="n">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="P6" t="n">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="Q6" t="n">
-        <v>1344</v>
+        <v>81</v>
+      </c>
+      <c r="R6" t="n">
+        <v>50</v>
+      </c>
+      <c r="S6" t="n">
+        <v>815</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>41791</v>
+        <v>44713</v>
       </c>
       <c r="B7" t="n">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C7" t="n">
-        <v>205</v>
+        <v>54</v>
       </c>
       <c r="D7" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E7" t="n">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="F7" t="n">
+        <v>19</v>
+      </c>
+      <c r="G7" t="n">
+        <v>46</v>
+      </c>
+      <c r="H7" t="n">
+        <v>25</v>
+      </c>
+      <c r="I7" t="n">
+        <v>48</v>
+      </c>
+      <c r="J7" t="n">
+        <v>61</v>
+      </c>
+      <c r="K7" t="n">
         <v>27</v>
       </c>
-      <c r="G7" t="n">
-        <v>60</v>
-      </c>
-      <c r="H7" t="n">
+      <c r="L7" t="n">
+        <v>57</v>
+      </c>
+      <c r="M7" t="n">
+        <v>12</v>
+      </c>
+      <c r="N7" t="n">
+        <v>59</v>
+      </c>
+      <c r="O7" t="n">
+        <v>62</v>
+      </c>
+      <c r="P7" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>90</v>
+      </c>
+      <c r="R7" t="n">
         <v>58</v>
       </c>
-      <c r="I7" t="n">
-        <v>55</v>
-      </c>
-      <c r="J7" t="n">
-        <v>175</v>
-      </c>
-      <c r="K7" t="n">
-        <v>43</v>
-      </c>
-      <c r="L7" t="n">
-        <v>194</v>
-      </c>
-      <c r="M7" t="n">
-        <v>32</v>
-      </c>
-      <c r="N7" t="n">
-        <v>61</v>
-      </c>
-      <c r="O7" t="n">
-        <v>126</v>
-      </c>
-      <c r="P7" t="n">
-        <v>89</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>1298</v>
+      <c r="S7" t="n">
+        <v>826</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>41821</v>
+        <v>44743</v>
       </c>
       <c r="B8" t="n">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C8" t="n">
-        <v>164</v>
+        <v>65</v>
       </c>
       <c r="D8" t="n">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E8" t="n">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="F8" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G8" t="n">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="H8" t="n">
+        <v>40</v>
+      </c>
+      <c r="I8" t="n">
+        <v>49</v>
+      </c>
+      <c r="J8" t="n">
         <v>60</v>
       </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
+        <v>29</v>
+      </c>
+      <c r="L8" t="n">
         <v>52</v>
       </c>
-      <c r="J8" t="n">
-        <v>206</v>
-      </c>
-      <c r="K8" t="n">
-        <v>38</v>
-      </c>
-      <c r="L8" t="n">
-        <v>137</v>
-      </c>
       <c r="M8" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="N8" t="n">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="O8" t="n">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="P8" t="n">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="Q8" t="n">
-        <v>1269</v>
+        <v>82</v>
+      </c>
+      <c r="R8" t="n">
+        <v>65</v>
+      </c>
+      <c r="S8" t="n">
+        <v>879</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>41852</v>
+        <v>44774</v>
       </c>
       <c r="B9" t="n">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C9" t="n">
-        <v>192</v>
+        <v>57</v>
       </c>
       <c r="D9" t="n">
+        <v>15</v>
+      </c>
+      <c r="E9" t="n">
+        <v>38</v>
+      </c>
+      <c r="F9" t="n">
+        <v>13</v>
+      </c>
+      <c r="G9" t="n">
+        <v>77</v>
+      </c>
+      <c r="H9" t="n">
         <v>29</v>
       </c>
-      <c r="E9" t="n">
-        <v>106</v>
-      </c>
-      <c r="F9" t="n">
-        <v>31</v>
-      </c>
-      <c r="G9" t="n">
-        <v>70</v>
-      </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
+        <v>51</v>
+      </c>
+      <c r="J9" t="n">
         <v>56</v>
       </c>
-      <c r="I9" t="n">
-        <v>34</v>
-      </c>
-      <c r="J9" t="n">
-        <v>151</v>
-      </c>
       <c r="K9" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="L9" t="n">
-        <v>169</v>
+        <v>52</v>
       </c>
       <c r="M9" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="N9" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O9" t="n">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="P9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="Q9" t="n">
-        <v>1249</v>
+        <v>73</v>
+      </c>
+      <c r="R9" t="n">
+        <v>65</v>
+      </c>
+      <c r="S9" t="n">
+        <v>837</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>41883</v>
+        <v>44805</v>
       </c>
       <c r="B10" t="n">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C10" t="n">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="D10" t="n">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E10" t="n">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="F10" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G10" t="n">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="H10" t="n">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="I10" t="n">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="J10" t="n">
-        <v>171</v>
+        <v>38</v>
       </c>
       <c r="K10" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="L10" t="n">
-        <v>144</v>
+        <v>41</v>
       </c>
       <c r="M10" t="n">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="N10" t="n">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="O10" t="n">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="P10" t="n">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="Q10" t="n">
-        <v>1264</v>
+        <v>67</v>
+      </c>
+      <c r="R10" t="n">
+        <v>64</v>
+      </c>
+      <c r="S10" t="n">
+        <v>806</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>41913</v>
+        <v>44835</v>
       </c>
       <c r="B11" t="n">
+        <v>33</v>
+      </c>
+      <c r="C11" t="n">
+        <v>62</v>
+      </c>
+      <c r="D11" t="n">
+        <v>15</v>
+      </c>
+      <c r="E11" t="n">
+        <v>44</v>
+      </c>
+      <c r="F11" t="n">
+        <v>22</v>
+      </c>
+      <c r="G11" t="n">
+        <v>36</v>
+      </c>
+      <c r="H11" t="n">
+        <v>38</v>
+      </c>
+      <c r="I11" t="n">
+        <v>37</v>
+      </c>
+      <c r="J11" t="n">
+        <v>50</v>
+      </c>
+      <c r="K11" t="n">
+        <v>30</v>
+      </c>
+      <c r="L11" t="n">
+        <v>51</v>
+      </c>
+      <c r="M11" t="n">
+        <v>15</v>
+      </c>
+      <c r="N11" t="n">
+        <v>56</v>
+      </c>
+      <c r="O11" t="n">
+        <v>63</v>
+      </c>
+      <c r="P11" t="n">
         <v>68</v>
       </c>
-      <c r="C11" t="n">
-        <v>157</v>
-      </c>
-      <c r="D11" t="n">
-        <v>28</v>
-      </c>
-      <c r="E11" t="n">
-        <v>89</v>
-      </c>
-      <c r="F11" t="n">
-        <v>37</v>
-      </c>
-      <c r="G11" t="n">
-        <v>55</v>
-      </c>
-      <c r="H11" t="n">
-        <v>36</v>
-      </c>
-      <c r="I11" t="n">
-        <v>48</v>
-      </c>
-      <c r="J11" t="n">
-        <v>161</v>
-      </c>
-      <c r="K11" t="n">
-        <v>44</v>
-      </c>
-      <c r="L11" t="n">
-        <v>134</v>
-      </c>
-      <c r="M11" t="n">
-        <v>29</v>
-      </c>
-      <c r="N11" t="n">
-        <v>58</v>
-      </c>
-      <c r="O11" t="n">
-        <v>145</v>
-      </c>
-      <c r="P11" t="n">
-        <v>89</v>
-      </c>
       <c r="Q11" t="n">
-        <v>1178</v>
+        <v>74</v>
+      </c>
+      <c r="R11" t="n">
+        <v>43</v>
+      </c>
+      <c r="S11" t="n">
+        <v>737</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>41944</v>
+        <v>44866</v>
       </c>
       <c r="B12" t="n">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C12" t="n">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="D12" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F12" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G12" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H12" t="n">
+        <v>22</v>
+      </c>
+      <c r="I12" t="n">
+        <v>26</v>
+      </c>
+      <c r="J12" t="n">
+        <v>35</v>
+      </c>
+      <c r="K12" t="n">
+        <v>20</v>
+      </c>
+      <c r="L12" t="n">
         <v>45</v>
-      </c>
-      <c r="I12" t="n">
-        <v>28</v>
-      </c>
-      <c r="J12" t="n">
-        <v>102</v>
-      </c>
-      <c r="K12" t="n">
-        <v>31</v>
-      </c>
-      <c r="L12" t="n">
-        <v>98</v>
       </c>
       <c r="M12" t="n">
         <v>10</v>
       </c>
       <c r="N12" t="n">
+        <v>38</v>
+      </c>
+      <c r="O12" t="n">
+        <v>67</v>
+      </c>
+      <c r="P12" t="n">
+        <v>69</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>48</v>
+      </c>
+      <c r="R12" t="n">
         <v>53</v>
       </c>
-      <c r="O12" t="n">
-        <v>75</v>
-      </c>
-      <c r="P12" t="n">
-        <v>65</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>816</v>
+      <c r="S12" t="n">
+        <v>635</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>41974</v>
+        <v>44896</v>
       </c>
       <c r="B13" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="n">
+        <v>21</v>
+      </c>
+      <c r="F13" t="n">
+        <v>12</v>
+      </c>
+      <c r="G13" t="n">
+        <v>40</v>
+      </c>
+      <c r="H13" t="n">
+        <v>23</v>
+      </c>
+      <c r="I13" t="n">
+        <v>22</v>
+      </c>
+      <c r="J13" t="n">
+        <v>23</v>
+      </c>
+      <c r="K13" t="n">
         <v>11</v>
       </c>
-      <c r="E13" t="n">
-        <v>47</v>
-      </c>
-      <c r="F13" t="n">
-        <v>5</v>
-      </c>
-      <c r="G13" t="n">
-        <v>20</v>
-      </c>
-      <c r="H13" t="n">
-        <v>21</v>
-      </c>
-      <c r="I13" t="n">
-        <v>19</v>
-      </c>
-      <c r="J13" t="n">
-        <v>71</v>
-      </c>
-      <c r="K13" t="n">
-        <v>14</v>
-      </c>
       <c r="L13" t="n">
-        <v>107</v>
+        <v>23</v>
       </c>
       <c r="M13" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="N13" t="n">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="O13" t="n">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="P13" t="n">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="Q13" t="n">
-        <v>584</v>
+        <v>38</v>
+      </c>
+      <c r="R13" t="n">
+        <v>26</v>
+      </c>
+      <c r="S13" t="n">
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>